<commit_message>
MAJ des tests faits
</commit_message>
<xml_diff>
--- a/Suivi des tests.xlsx
+++ b/Suivi des tests.xlsx
@@ -13,6 +13,47 @@
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+  <si>
+    <t>post avec un ticket test</t>
+  </si>
+  <si>
+    <t>réussi</t>
+  </si>
+  <si>
+    <t>echec</t>
+  </si>
+  <si>
+    <t>réussite après modif: validation des donnes et types</t>
+  </si>
+  <si>
+    <t>sur le site (avant cypress)</t>
+  </si>
+  <si>
+    <t>pas de methode fetch</t>
+  </si>
+  <si>
+    <t>Bdd sqlite 1</t>
+  </si>
+  <si>
+    <t>Bdd sqlite 2</t>
+  </si>
+  <si>
+    <t>objet</t>
+  </si>
+  <si>
+    <t>résultat</t>
+  </si>
+  <si>
+    <t>causes possibles</t>
+  </si>
+  <si>
+    <t>erreur dans le code ?</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -342,12 +383,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
fonctionnalités testes, tris asc dec ok add ticket ok / reste à revoir
</commit_message>
<xml_diff>
--- a/Suivi des tests.xlsx
+++ b/Suivi des tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>post avec un ticket test</t>
   </si>
@@ -33,9 +33,6 @@
     <t>sur le site (avant cypress)</t>
   </si>
   <si>
-    <t>pas de methode fetch</t>
-  </si>
-  <si>
     <t>Bdd sqlite 1</t>
   </si>
   <si>
@@ -52,6 +49,45 @@
   </si>
   <si>
     <t>erreur dans le code ?</t>
+  </si>
+  <si>
+    <t>lien bdd site ok</t>
+  </si>
+  <si>
+    <t>lien routes bdd ok mais formulaire bdd non</t>
+  </si>
+  <si>
+    <t>liste des tickets à afficher</t>
+  </si>
+  <si>
+    <t>pas de methode fetch =&gt; réécriture des fonctions. Deplus app,js inexistant</t>
+  </si>
+  <si>
+    <t>tri asc</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>tri desc</t>
+  </si>
+  <si>
+    <t>autres tris</t>
+  </si>
+  <si>
+    <t>[] (vide)</t>
+  </si>
+  <si>
+    <t>del</t>
+  </si>
+  <si>
+    <t>selection par id à revoir</t>
+  </si>
+  <si>
+    <t>update</t>
+  </si>
+  <si>
+    <t>à faire</t>
   </si>
 </sst>
 </file>
@@ -383,30 +419,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -414,26 +452,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -441,7 +482,56 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout des dernières modifications, readme a terminer (liste html)
</commit_message>
<xml_diff>
--- a/Suivi des tests.xlsx
+++ b/Suivi des tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>post avec un ticket test</t>
   </si>
@@ -428,7 +428,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -498,6 +498,9 @@
       </c>
     </row>
     <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
       <c r="B6" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
suivi des test terminé
</commit_message>
<xml_diff>
--- a/Suivi des tests.xlsx
+++ b/Suivi des tests.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="23655" windowHeight="10500"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="23655" windowHeight="10500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="unitaires" sheetId="1" r:id="rId1"/>
+    <sheet name="integration" sheetId="4" r:id="rId2"/>
+    <sheet name="Acceptation" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
   <si>
     <t>post avec un ticket test</t>
   </si>
@@ -30,15 +30,6 @@
     <t>réussite après modif: validation des donnes et types</t>
   </si>
   <si>
-    <t>sur le site (avant cypress)</t>
-  </si>
-  <si>
-    <t>Bdd sqlite 1</t>
-  </si>
-  <si>
-    <t>Bdd sqlite 2</t>
-  </si>
-  <si>
     <t>objet</t>
   </si>
   <si>
@@ -54,12 +45,6 @@
     <t>lien bdd site ok</t>
   </si>
   <si>
-    <t>lien routes bdd ok mais formulaire bdd non</t>
-  </si>
-  <si>
-    <t>liste des tickets à afficher</t>
-  </si>
-  <si>
     <t>pas de methode fetch =&gt; réécriture des fonctions. Deplus app,js inexistant</t>
   </si>
   <si>
@@ -72,35 +57,119 @@
     <t>tri desc</t>
   </si>
   <si>
-    <t>autres tris</t>
-  </si>
-  <si>
     <t>[] (vide)</t>
   </si>
   <si>
-    <t>del</t>
-  </si>
-  <si>
     <t>selection par id à revoir</t>
   </si>
   <si>
     <t>update</t>
   </si>
   <si>
-    <t>à faire</t>
-  </si>
-  <si>
     <t>reussite</t>
   </si>
   <si>
     <t>/ dans la position des css et js manquant (il comprenais/api/…)</t>
+  </si>
+  <si>
+    <t>incompréhension initiale avec les routes et les?</t>
+  </si>
+  <si>
+    <t>responsive</t>
+  </si>
+  <si>
+    <t>plusieurs essais pour y arriver</t>
+  </si>
+  <si>
+    <t>autres notes</t>
+  </si>
+  <si>
+    <t>lien routes bdd ok mais formulaire bdd non, liste des tickets à afficher</t>
+  </si>
+  <si>
+    <t>action de remplissage du formulaire complet</t>
+  </si>
+  <si>
+    <t>action de remplissage du formulaire incomplet</t>
+  </si>
+  <si>
+    <t>tri asc (postman)</t>
+  </si>
+  <si>
+    <t>tri desc (postman)</t>
+  </si>
+  <si>
+    <t>mise a jour</t>
+  </si>
+  <si>
+    <t>suppression</t>
+  </si>
+  <si>
+    <t>filtre par titre</t>
+  </si>
+  <si>
+    <t>filtre par autheur</t>
+  </si>
+  <si>
+    <t>filtre par priorité</t>
+  </si>
+  <si>
+    <t>filtre par status</t>
+  </si>
+  <si>
+    <t>axes d'amélioration</t>
+  </si>
+  <si>
+    <t>ajouter des comptes admins</t>
+  </si>
+  <si>
+    <t>restreindre les permissions de suppression aux admins</t>
+  </si>
+  <si>
+    <t>ajout du ticket</t>
+  </si>
+  <si>
+    <t>token jwt pour l'etat restless / acces 1h (impact d'atk dessus à calculer)</t>
+  </si>
+  <si>
+    <t>accès à la Bdd sqlite 1</t>
+  </si>
+  <si>
+    <t>accès à laBdd sqlite 2</t>
+  </si>
+  <si>
+    <t>del 2 (postman)</t>
+  </si>
+  <si>
+    <t>del 1 (postman)</t>
+  </si>
+  <si>
+    <t>autres tris 1 (postman)</t>
+  </si>
+  <si>
+    <t>autres tris 2 (postman)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sur le site </t>
+  </si>
+  <si>
+    <t>sur le site</t>
+  </si>
+  <si>
+    <t>au 1er essais les boutons ne réagissaient pas à cause d'erreurs dans les fonctions, le js</t>
+  </si>
+  <si>
+    <t>il précise bien que les champs sont obligatoires</t>
+  </si>
+  <si>
+    <t>il confirme l'entrée du ticket</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,16 +177,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -125,12 +239,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,157 +567,443 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="68" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="18">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="C11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="B13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+      <c r="B14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
+      <c r="D14" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="10" customFormat="1" ht="18">
+      <c r="A1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="7"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajout de boutons spécifiques aux tickets pour supprimmer et modifier ; modifications des retours (500 / 400 , 200 / 201) dans routes.js. Il va falloir lancer les tests unitaires (JEST), d'intégration (Newman avec itérations) et fonctionnels (avec CYPRESS).
</commit_message>
<xml_diff>
--- a/Suivi des tests.xlsx
+++ b/Suivi des tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
   <si>
     <t>post avec un ticket test</t>
   </si>
@@ -120,18 +120,9 @@
     <t>axes d'amélioration</t>
   </si>
   <si>
-    <t>ajouter des comptes admins</t>
-  </si>
-  <si>
-    <t>restreindre les permissions de suppression aux admins</t>
-  </si>
-  <si>
     <t>ajout du ticket</t>
   </si>
   <si>
-    <t>token jwt pour l'etat restless / acces 1h (impact d'atk dessus à calculer)</t>
-  </si>
-  <si>
     <t>accès à la Bdd sqlite 1</t>
   </si>
   <si>
@@ -163,6 +154,27 @@
   </si>
   <si>
     <t>il confirme l'entrée du ticket</t>
+  </si>
+  <si>
+    <t>Ajouter des comptes admins</t>
+  </si>
+  <si>
+    <t>Restreindre les permissions de suppression aux admins</t>
+  </si>
+  <si>
+    <t>Token jwt pour l'etat restless / acces 1h (impact d'atk dessus à calculer)</t>
+  </si>
+  <si>
+    <t>Tests automatisés pour les test de regression (après maj d'ajout de fonctionnalités) avec cypress, newman</t>
+  </si>
+  <si>
+    <t>add ticket avec toutes prioritées, upddate avec open close et in_progress</t>
+  </si>
+  <si>
+    <t>tickets complets et incompletes avec 3 auteurs</t>
+  </si>
+  <si>
+    <t>tout supprimer à la fin</t>
   </si>
 </sst>
 </file>
@@ -187,7 +199,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,6 +242,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -258,10 +276,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -273,6 +290,18 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,179 +604,179 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="68" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="64" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="18">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="18">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="11"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="7" t="s">
+      <c r="C11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="7"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="7" t="s">
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="7" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -771,136 +800,136 @@
     <col min="4" max="4" width="43.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="10" customFormat="1" ht="18">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:5" s="9" customFormat="1" ht="18">
+      <c r="A1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="9"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7" t="s">
-        <v>48</v>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7" t="s">
-        <v>47</v>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="7"/>
+      <c r="C6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="7"/>
+      <c r="C7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="7"/>
+      <c r="C8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="7"/>
+      <c r="C9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="7"/>
+      <c r="C10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="7"/>
+      <c r="C11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -909,99 +938,182 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" s="15" t="s">
         <v>23</v>
       </c>
+      <c r="C2" s="16"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
+      <c r="C3" s="16"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="A4" s="15" t="s">
         <v>10</v>
       </c>
+      <c r="C4" s="16"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="A5" s="15" t="s">
         <v>12</v>
       </c>
+      <c r="C5" s="16"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" t="s">
+      <c r="A6" s="15" t="s">
         <v>27</v>
       </c>
+      <c r="C6" s="16"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" t="s">
+      <c r="A7" s="15" t="s">
         <v>28</v>
       </c>
+      <c r="C7" s="16"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" t="s">
+      <c r="A8" s="15" t="s">
         <v>29</v>
       </c>
+      <c r="C8" s="16"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" t="s">
+      <c r="A9" s="15" t="s">
         <v>30</v>
       </c>
+      <c r="C9" s="16"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" t="s">
+      <c r="A10" s="15" t="s">
         <v>31</v>
       </c>
+      <c r="C10" s="16"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" t="s">
+      <c r="A11" s="15" t="s">
         <v>32</v>
       </c>
+      <c r="C11" s="16"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>36</v>
-      </c>
+      <c r="A12" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="16"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="15"/>
+      <c r="C13" s="16"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="C14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="C15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="C16" t="s">
-        <v>37</v>
-      </c>
+      <c r="A14" s="15"/>
+      <c r="C14" s="16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30">
+      <c r="A15" s="15"/>
+      <c r="C15" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30">
+      <c r="A16" s="15"/>
+      <c r="C16" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="45">
+      <c r="A17" s="15"/>
+      <c r="C17" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30">
+      <c r="A18" s="15"/>
+      <c r="C18" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30">
+      <c r="A19" s="15"/>
+      <c r="C19" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="15"/>
+      <c r="C20" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="15"/>
+      <c r="C21" s="16"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="15"/>
+      <c r="C22" s="16"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="15"/>
+      <c r="C23" s="16"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="15"/>
+      <c r="C24" s="16"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="15"/>
+      <c r="C25" s="16"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="15"/>
+      <c r="C26" s="16"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="15"/>
+      <c r="C27" s="16"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="15"/>
+      <c r="C28" s="16"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="15"/>
+      <c r="C29" s="16"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="15"/>
+      <c r="C30" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>